<commit_message>
Draft shared with Janneke! Making progress ... but soon I must face the personal data form (booh, sad face).
</commit_message>
<xml_diff>
--- a/budget/nerscalliancesnsf2024budget.xlsx
+++ b/budget/nerscalliancesnsf2024budget.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/grants/nserc/nsercalliancesnsf2024/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C57F4A-0AC4-BF47-8E0A-41D2EBADD452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD64784E-644B-0542-ABD0-5981ED11971D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="3140" windowWidth="27640" windowHeight="16940" xr2:uid="{DD0427ED-F24A-0447-A744-331E96372E50}"/>
+    <workbookView xWindow="22180" yWindow="4880" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{DD0427ED-F24A-0447-A744-331E96372E50}"/>
   </bookViews>
   <sheets>
-    <sheet name="ubc_budget" sheetId="1" r:id="rId1"/>
-    <sheet name="meta" sheetId="2" r:id="rId2"/>
+    <sheet name="ubcbudget" sheetId="1" r:id="rId1"/>
+    <sheet name="ethbudget_nsercformat" sheetId="3" r:id="rId2"/>
+    <sheet name="meta" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="133">
   <si>
     <t>Year</t>
   </si>
@@ -131,9 +132,6 @@
     <t>Budget for NSERC Alliance</t>
   </si>
   <si>
-    <t>Based off budgetalternative tab in mountrainierlogistics/grants/snsf2024/notposting/budgetme/snsf2024_wolkovichbudget.xlsx -- CHECK OUT that sheet for more info</t>
-  </si>
-  <si>
     <t>See the budget justification for an explanation of costs.</t>
   </si>
   <si>
@@ -144,13 +142,314 @@
   </si>
   <si>
     <t>Travel for something</t>
+  </si>
+  <si>
+    <t>ubcbudget tab is based off budgetalternative tab in mountrainierlogistics/grants/snsf2024/notposting/budgetme/snsf2024_wolkovichbudget.xlsx -- CHECK OUT that sheet for more info</t>
+  </si>
+  <si>
+    <t>ethbudget_nsercformat tab created from nsercalliancesnsf2024/notposting/snsf/Budget_SNF_Apr.2024.xlsx</t>
+  </si>
+  <si>
+    <t>BUDGET SNF</t>
+  </si>
+  <si>
+    <t>SALARY / PEOPLE</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Salary &amp; Social Security</t>
+  </si>
+  <si>
+    <t>Percent 2025</t>
+  </si>
+  <si>
+    <t># Items 2026</t>
+  </si>
+  <si>
+    <t># Items 2027</t>
+  </si>
+  <si>
+    <t>Cost 2025</t>
+  </si>
+  <si>
+    <t>Cost 2026</t>
+  </si>
+  <si>
+    <t>Cost 2027</t>
+  </si>
+  <si>
+    <t>Line total</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>NSERC equivalent?</t>
+  </si>
+  <si>
+    <t>Postdoc</t>
+  </si>
+  <si>
+    <t>Pathogens</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Graduate Student</t>
+  </si>
+  <si>
+    <t>Seed predation</t>
+  </si>
+  <si>
+    <t>Masters student + Mao (funded by Wolkovich)</t>
+  </si>
+  <si>
+    <t>First 1.5 years from HRL budget</t>
+  </si>
+  <si>
+    <t>50 Percent field assistant</t>
+  </si>
+  <si>
+    <t>help with pathogens, seed predation (in US)</t>
+  </si>
+  <si>
+    <t>50% paid from HRL budget</t>
+  </si>
+  <si>
+    <t>Hilfassistenten</t>
+  </si>
+  <si>
+    <t>UBC undergrads</t>
+  </si>
+  <si>
+    <t>Seed sorting hilf assistenten paid from HRL budget</t>
+  </si>
+  <si>
+    <t>TOTAL SALARIES &amp; SS Security</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Costs (per item)</t>
+  </si>
+  <si>
+    <t># Items 2025</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Needed for</t>
+  </si>
+  <si>
+    <t>Car (CH)</t>
+  </si>
+  <si>
+    <t>Car (USA)</t>
+  </si>
+  <si>
+    <t>NSERC field travel</t>
+  </si>
+  <si>
+    <t>Flights to USA / Meetings</t>
+  </si>
+  <si>
+    <t>Conferences, team meetings for UBC team</t>
+  </si>
+  <si>
+    <t>Housing (USA)</t>
+  </si>
+  <si>
+    <t>While visiting US field sites, a car is needed (the field sites are 150 km from Seattle, with no reliable public transportation). For 1.5 month car rental and gas, this is approximately $3000. Lodging is additionally needed for the PI (for 2 weeks), the graduate student and/or the postdoc (both in year 2 - for 6 weeks). Lodging is a combination of field house lodging provided by Mt. Rainier NP (25$ per person per night), nearby motels (~80$ per person per night), and Airbnb (~$250 for a team of 3 per night). From experience, these costs will likely reach &gt;$9000. Any additional costs incurred will be covered by the budget of PI Hille Ris Lambers.</t>
+  </si>
+  <si>
+    <t>Housing for UBC team</t>
+  </si>
+  <si>
+    <t>Field Food (CH)</t>
+  </si>
+  <si>
+    <t>Food for UBC team</t>
+  </si>
+  <si>
+    <t>Field Food (USA)</t>
+  </si>
+  <si>
+    <t>Conference (travel, food, hotel, registration)</t>
+  </si>
+  <si>
+    <t>TOTAL TRAVEL</t>
+  </si>
+  <si>
+    <t>Supplies and consumables</t>
+  </si>
+  <si>
+    <t>Field supplies - regeneration monitoring</t>
+  </si>
+  <si>
+    <t>Replacement microclimate sensors, seed traps, etc</t>
+  </si>
+  <si>
+    <t>none (funded by HRL)</t>
+  </si>
+  <si>
+    <t>Covered by HRL budget</t>
+  </si>
+  <si>
+    <t>Field supplies - seed predation (CH)</t>
+  </si>
+  <si>
+    <t>Seed trays, boxes, paper bags, sand, etc</t>
+  </si>
+  <si>
+    <t>USA on NSERC</t>
+  </si>
+  <si>
+    <t>Lab supplies - seed pathogens (CH)</t>
+  </si>
+  <si>
+    <t>Soil, germination boxes, etc</t>
+  </si>
+  <si>
+    <t>Camera Traps - CH</t>
+  </si>
+  <si>
+    <t>Capturing seed predators in stands</t>
+  </si>
+  <si>
+    <t>Could be covered by HRL ETH budget</t>
+  </si>
+  <si>
+    <t>Seeds (CH)</t>
+  </si>
+  <si>
+    <t>For predation trials, pathogen trials</t>
+  </si>
+  <si>
+    <t>Kits for DNA extraction (QiaGen)</t>
+  </si>
+  <si>
+    <t>Powermax - DNeasy kit for soil - 250 samples. find on ethis</t>
+  </si>
+  <si>
+    <t>USA on NSERC - need about 378 if go for 6 stands (yikes).</t>
+  </si>
+  <si>
+    <t>Glassware</t>
+  </si>
+  <si>
+    <t>Amplicon Library &amp; Sequencing</t>
+  </si>
+  <si>
+    <t>5500 for 384 samples, so need 4 per year to get to 1200. Add a 10% buffer for glassware</t>
+  </si>
+  <si>
+    <t>Go for 1000 trays? Smaller trays</t>
+  </si>
+  <si>
+    <t>Custom primers, prep, glassware</t>
+  </si>
+  <si>
+    <t>Sequencing cost per sample, includes bioinformatics. add 30% for errors</t>
+  </si>
+  <si>
+    <t>TOTAL MATERIALS AND SUPPLIES</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>Mort classes (high, low)</t>
+  </si>
+  <si>
+    <t>no postdoc</t>
+  </si>
+  <si>
+    <t>Reps</t>
+  </si>
+  <si>
+    <t>collect soils - save? Hope we find someone?</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Types DNA</t>
+  </si>
+  <si>
+    <t>Samples per year</t>
+  </si>
+  <si>
+    <t>Contributions from Partner organization:</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>equipment/software</t>
+  </si>
+  <si>
+    <t>materials</t>
+  </si>
+  <si>
+    <t>field work logistics</t>
+  </si>
+  <si>
+    <t>provision of services</t>
+  </si>
+  <si>
+    <t>use of organization's facilities</t>
+  </si>
+  <si>
+    <t>salaeries of admin staff</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Funded is 450,000</t>
+  </si>
+  <si>
+    <t>Cut:</t>
+  </si>
+  <si>
+    <t>New!</t>
+  </si>
+  <si>
+    <t>NSERC form requires organization into these categories by Year:</t>
+  </si>
+  <si>
+    <t>Cut options: MV Eleanore to other funds; cut field assistant brings us close</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -173,13 +472,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C6E7"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -194,15 +559,94 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -514,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD7B1CE-8F13-8B46-83A7-00F602A9A8B4}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,7 +1005,7 @@
         <v>34000</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2">
         <f>C2-7000</f>
@@ -775,14 +1219,14 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>3500</v>
+        <v>11000</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f>C11*D11</f>
-        <v>10500</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -790,17 +1234,17 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>3500</v>
+        <v>3000</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
         <f>C12*D12</f>
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -847,7 +1291,7 @@
         <v>103.16</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -961,33 +1405,1395 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFCABA2-8D40-B74F-944B-94AF5E91C8C5}">
+  <dimension ref="A1:W45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J2" s="7"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="5">
+        <f>R9</f>
+        <v>659414.99199999997</v>
+      </c>
+      <c r="F5" s="26">
+        <f>E5-E14</f>
+        <v>360845</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="4">
+        <v>112403.99999999999</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="9">
+        <v>1</v>
+      </c>
+      <c r="N5" s="9">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>56201.999999999993</v>
+      </c>
+      <c r="P5" s="4">
+        <v>112403.99999999999</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>112403.99999999999</v>
+      </c>
+      <c r="R5" s="10">
+        <v>281009.99999999994</v>
+      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="4">
+        <v>60366.399999999994</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
+        <v>1</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="4">
+        <v>60366.399999999994</v>
+      </c>
+      <c r="P6" s="4">
+        <v>60366.399999999994</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>30183.199999999997</v>
+      </c>
+      <c r="R6" s="5">
+        <v>150916</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="18">
+        <v>62655</v>
+      </c>
+      <c r="F7" s="18">
+        <v>62655</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="4">
+        <v>92800</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="4">
+        <v>46400</v>
+      </c>
+      <c r="P7" s="4">
+        <v>46400</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>46400</v>
+      </c>
+      <c r="R7" s="10">
+        <v>139200</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="4">
+        <v>73574.159999999989</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="O8" s="4">
+        <v>29429.663999999997</v>
+      </c>
+      <c r="P8" s="4">
+        <v>29429.663999999997</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>29429.663999999997</v>
+      </c>
+      <c r="R8" s="10">
+        <v>88288.991999999998</v>
+      </c>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="5">
+        <v>659414.99199999997</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="4"/>
+      <c r="T11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="V11" s="4"/>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="16">
+        <v>26500</v>
+      </c>
+      <c r="F12" s="16">
+        <v>26500</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="11">
+        <v>500</v>
+      </c>
+      <c r="L12" s="13">
+        <v>6</v>
+      </c>
+      <c r="M12" s="13">
+        <v>6</v>
+      </c>
+      <c r="N12" s="13">
+        <v>6</v>
+      </c>
+      <c r="O12" s="4">
+        <v>3000</v>
+      </c>
+      <c r="P12" s="4">
+        <v>3000</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>3000</v>
+      </c>
+      <c r="R12" s="5">
+        <v>9000</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="V12" s="4"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="26">
+        <f>SUM(E5:E12)</f>
+        <v>748569.99199999997</v>
+      </c>
+      <c r="F13" s="26">
+        <f>SUM(F5:F12)</f>
+        <v>450000</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="11">
+        <v>1000</v>
+      </c>
+      <c r="L13" s="13">
+        <v>2</v>
+      </c>
+      <c r="M13" s="13">
+        <v>2</v>
+      </c>
+      <c r="N13" s="13">
+        <v>2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2000</v>
+      </c>
+      <c r="P13" s="4">
+        <v>2000</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2000</v>
+      </c>
+      <c r="R13" s="14">
+        <v>0</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V13" s="4"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="26">
+        <f>E13-450000</f>
+        <v>298569.99199999997</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="11">
+        <v>1000</v>
+      </c>
+      <c r="L14" s="13">
+        <v>2</v>
+      </c>
+      <c r="M14" s="13">
+        <v>3</v>
+      </c>
+      <c r="N14" s="13">
+        <v>2</v>
+      </c>
+      <c r="O14" s="4">
+        <v>2000</v>
+      </c>
+      <c r="P14" s="4">
+        <v>3000</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>2000</v>
+      </c>
+      <c r="R14" s="5">
+        <v>7000</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="V14" s="4"/>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="11">
+        <v>1275</v>
+      </c>
+      <c r="L15" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="M15" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="N15" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="O15" s="4">
+        <v>3187.5</v>
+      </c>
+      <c r="P15" s="4">
+        <v>3187.5</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>3187.5</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V15" s="4"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="26">
+        <f>SUM(R6:R7)</f>
+        <v>290116</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="15">
+        <v>250</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="V16" s="4"/>
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="11">
+        <v>580</v>
+      </c>
+      <c r="L17" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="M17" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="N17" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1450</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1450</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>1450</v>
+      </c>
+      <c r="R17" s="14">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="V17" s="4"/>
+      <c r="W17" s="6"/>
+    </row>
+    <row r="18" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="15">
+        <v>1500</v>
+      </c>
+      <c r="L18" s="15">
+        <v>2</v>
+      </c>
+      <c r="M18" s="15">
+        <v>3</v>
+      </c>
+      <c r="N18" s="15">
+        <v>2</v>
+      </c>
+      <c r="O18" s="4">
+        <v>3000</v>
+      </c>
+      <c r="P18" s="4">
+        <v>4500</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>3000</v>
+      </c>
+      <c r="R18" s="5">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="19" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J19" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="R19" s="16">
+        <v>26500</v>
+      </c>
+    </row>
+    <row r="20" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J20" s="7"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S21" s="4"/>
+      <c r="T21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="11">
+        <v>10000</v>
+      </c>
+      <c r="L22" s="5">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0</v>
+      </c>
+      <c r="R22" s="17">
+        <v>0</v>
+      </c>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="11">
+        <v>3000</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O23" s="4">
+        <v>3000</v>
+      </c>
+      <c r="P23" s="4">
+        <v>1500</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>1500</v>
+      </c>
+      <c r="R23" s="4">
+        <v>6000</v>
+      </c>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V23" s="4"/>
+      <c r="W23" s="6"/>
+    </row>
+    <row r="24" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J24" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="11">
+        <v>3000</v>
+      </c>
+      <c r="L24" s="5">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O24" s="4">
+        <v>3000</v>
+      </c>
+      <c r="P24" s="4">
+        <v>1500</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>1500</v>
+      </c>
+      <c r="R24" s="4">
+        <v>6000</v>
+      </c>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V24" s="4"/>
+      <c r="W24" s="6"/>
+    </row>
+    <row r="25" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="11">
+        <v>6000</v>
+      </c>
+      <c r="L25" s="5">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0</v>
+      </c>
+      <c r="O25" s="4">
+        <v>6000</v>
+      </c>
+      <c r="P25" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>0</v>
+      </c>
+      <c r="R25" s="17">
+        <v>0</v>
+      </c>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="W25" s="6"/>
+    </row>
+    <row r="26" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" s="4">
+        <v>1000</v>
+      </c>
+      <c r="L26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26" s="4">
+        <v>1</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1</v>
+      </c>
+      <c r="O26" s="4">
+        <v>1000</v>
+      </c>
+      <c r="P26" s="4">
+        <v>1000</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>1000</v>
+      </c>
+      <c r="R26" s="17">
+        <v>0</v>
+      </c>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V26" s="4"/>
+      <c r="W26" s="6"/>
+    </row>
+    <row r="27" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K27" s="11">
+        <v>2350</v>
+      </c>
+      <c r="L27" s="11">
+        <v>0</v>
+      </c>
+      <c r="M27" s="11">
+        <v>0</v>
+      </c>
+      <c r="N27" s="11">
+        <v>3</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>7050</v>
+      </c>
+      <c r="R27" s="4">
+        <v>7050</v>
+      </c>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="U27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="V27" s="4"/>
+      <c r="W27" s="6"/>
+    </row>
+    <row r="28" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J28" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="K28" s="11">
+        <v>235</v>
+      </c>
+      <c r="L28" s="11">
+        <v>0</v>
+      </c>
+      <c r="M28" s="11">
+        <v>0</v>
+      </c>
+      <c r="N28" s="11">
+        <v>3</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>705</v>
+      </c>
+      <c r="R28" s="4">
+        <v>705</v>
+      </c>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+    </row>
+    <row r="29" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J29" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="K29" s="11">
+        <v>5500</v>
+      </c>
+      <c r="L29" s="11">
+        <v>0</v>
+      </c>
+      <c r="M29" s="11">
+        <v>0</v>
+      </c>
+      <c r="N29" s="11">
+        <v>6</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>33000</v>
+      </c>
+      <c r="R29" s="4">
+        <v>33000</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="U29" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J30" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="K30" s="18">
+        <v>1650</v>
+      </c>
+      <c r="L30" s="18">
+        <v>0</v>
+      </c>
+      <c r="M30" s="18">
+        <v>0</v>
+      </c>
+      <c r="N30" s="18">
+        <v>6</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>9900</v>
+      </c>
+      <c r="R30" s="4">
+        <v>9900</v>
+      </c>
+      <c r="S30" s="15">
+        <v>42900</v>
+      </c>
+      <c r="T30" s="15"/>
+    </row>
+    <row r="31" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="T31" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J32" s="12"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+    </row>
+    <row r="33" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J33" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18">
+        <v>62655</v>
+      </c>
+    </row>
+    <row r="34" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J34" s="19"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="U34" s="4">
+        <v>3</v>
+      </c>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+    </row>
+    <row r="35" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J35" s="19"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="U35" s="11">
+        <v>5</v>
+      </c>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+    </row>
+    <row r="36" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J36" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="K36" s="20"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22">
+        <v>748569.99199999997</v>
+      </c>
+      <c r="S36" s="20"/>
+      <c r="T36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="U36" s="4">
+        <v>3</v>
+      </c>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+    </row>
+    <row r="37" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J37" s="19"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="U37" s="4">
+        <v>2</v>
+      </c>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+    </row>
+    <row r="38" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J38" s="19"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22">
+        <v>467559.99200000003</v>
+      </c>
+      <c r="S38" s="20"/>
+      <c r="T38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="U38" s="4">
+        <v>3</v>
+      </c>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+    </row>
+    <row r="39" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J39" s="23"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="U39" s="4">
+        <v>2</v>
+      </c>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J40" s="23"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="U40" s="4">
+        <v>2</v>
+      </c>
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+    </row>
+    <row r="41" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J41" s="23"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+    </row>
+    <row r="42" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J42" s="23"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="U42" s="6">
+        <v>360</v>
+      </c>
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+    </row>
+    <row r="43" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J43" s="23"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="25"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
+      <c r="U43" s="6"/>
+      <c r="V43" s="6"/>
+      <c r="W43" s="6"/>
+    </row>
+    <row r="44" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J44" s="23"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+    </row>
+    <row r="45" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J45" s="23"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="R36">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>750000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+      <formula>750000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68B4139-A784-DE41-8066-804A424F12C4}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>32</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bunch of crazed work, so sick of this
</commit_message>
<xml_diff>
--- a/budget/nerscalliancesnsf2024budget.xlsx
+++ b/budget/nerscalliancesnsf2024budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/grants/nserc/nsercalliancesnsf2024/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80228AAC-92C5-FD47-B9EC-C5CDD7417270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01822993-2925-6843-95B6-27DC345C1E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1760" windowWidth="40640" windowHeight="21960" activeTab="1" xr2:uid="{DD0427ED-F24A-0447-A744-331E96372E50}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20360" windowHeight="17420" xr2:uid="{DD0427ED-F24A-0447-A744-331E96372E50}"/>
   </bookViews>
   <sheets>
     <sheet name="ubcbudget" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="146">
   <si>
     <t>Year</t>
   </si>
@@ -465,12 +465,24 @@
   <si>
     <t>Contributions from Partner organization: in CAD</t>
   </si>
+  <si>
+    <t>DOUBLE CHECK:</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>Student cost</t>
+  </si>
+  <si>
+    <t>Total students</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -575,8 +587,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,6 +624,12 @@
         <bgColor rgb="FFB4C6E7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -608,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -683,6 +718,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,15 +1068,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD7B1CE-8F13-8B46-83A7-00F602A9A8B4}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1060,8 +1098,24 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N1" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" t="s">
+        <v>143</v>
+      </c>
+      <c r="T1" t="s">
+        <v>144</v>
+      </c>
+      <c r="U1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1088,8 +1142,23 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1120,8 +1189,23 @@
       <c r="J3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N3" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="31">
+        <v>34000</v>
+      </c>
+      <c r="Q3" s="31">
+        <v>1</v>
+      </c>
+      <c r="R3" s="31">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1144,8 +1228,23 @@
       <c r="J4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N4" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="31">
+        <v>42.734999999999999</v>
+      </c>
+      <c r="Q4" s="31">
+        <v>680</v>
+      </c>
+      <c r="R4" s="32">
+        <v>29059.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1174,8 +1273,23 @@
       <c r="J5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="31">
+        <v>1700</v>
+      </c>
+      <c r="Q5" s="31">
+        <v>1</v>
+      </c>
+      <c r="R5" s="31">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1198,16 +1312,58 @@
       <c r="J6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="31">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="31">
+        <v>2480</v>
+      </c>
+      <c r="R6" s="31">
+        <v>32240</v>
+      </c>
+      <c r="S6">
+        <f>(4*4*35)+(4*24*20)</f>
+        <v>2480</v>
+      </c>
+      <c r="T6">
+        <f>13*S6</f>
+        <v>32240</v>
+      </c>
+      <c r="U6">
+        <f>SUM(R3,R6)</f>
+        <v>66240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="I7">
         <v>20</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="31">
+        <v>3000</v>
+      </c>
+      <c r="Q7" s="31">
+        <v>1</v>
+      </c>
+      <c r="R7" s="31">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1230,8 +1386,13 @@
       <c r="J8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1254,8 +1415,23 @@
       <c r="J9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="31">
+        <v>34000</v>
+      </c>
+      <c r="Q9" s="31">
+        <v>1</v>
+      </c>
+      <c r="R9" s="31">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1284,8 +1460,23 @@
       <c r="J10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N10" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="31">
+        <v>1400</v>
+      </c>
+      <c r="Q10" s="31">
+        <v>1</v>
+      </c>
+      <c r="R10" s="31">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1302,8 +1493,35 @@
         <f t="shared" si="0"/>
         <v>11000</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N11" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="31">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="31">
+        <v>3120</v>
+      </c>
+      <c r="R11" s="31">
+        <v>40560</v>
+      </c>
+      <c r="S11">
+        <f>4*4*35+4*24*20+8*4*20</f>
+        <v>3120</v>
+      </c>
+      <c r="T11">
+        <f>13*S11</f>
+        <v>40560</v>
+      </c>
+      <c r="U11">
+        <f>SUM(R11,R9)</f>
+        <v>74560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1320,8 +1538,23 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" s="31">
+        <v>11000</v>
+      </c>
+      <c r="Q12" s="31">
+        <v>1</v>
+      </c>
+      <c r="R12" s="31">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1338,8 +1571,40 @@
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N13" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="31">
+        <v>3000</v>
+      </c>
+      <c r="Q13" s="31">
+        <v>1</v>
+      </c>
+      <c r="R13" s="31">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N14" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="31">
+        <v>10000</v>
+      </c>
+      <c r="Q14" s="31">
+        <v>1</v>
+      </c>
+      <c r="R14" s="31">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1367,8 +1632,13 @@
       <c r="I15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1391,8 +1661,23 @@
         <f>3*4*35+3*32*20</f>
         <v>2340</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N16" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" s="31">
+        <v>103.16</v>
+      </c>
+      <c r="Q16" s="31">
+        <v>500</v>
+      </c>
+      <c r="R16" s="31">
+        <v>51580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1409,8 +1694,31 @@
         <f>C17*D17</f>
         <v>10500</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N17" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="31">
+        <v>13</v>
+      </c>
+      <c r="Q17" s="31">
+        <v>2340</v>
+      </c>
+      <c r="R17" s="31">
+        <v>30420</v>
+      </c>
+      <c r="S17">
+        <f>(3*4*35)+(32*20*3)</f>
+        <v>2340</v>
+      </c>
+      <c r="T17">
+        <f>13*S17</f>
+        <v>30420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1427,50 +1735,140 @@
         <f>C18*D18</f>
         <v>7500</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N18" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="P18" s="31">
+        <v>3500</v>
+      </c>
+      <c r="Q18" s="31">
+        <v>3</v>
+      </c>
+      <c r="R18" s="31">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I19" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N19" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" s="31">
+        <v>7500</v>
+      </c>
+      <c r="Q19" s="31">
+        <v>1</v>
+      </c>
+      <c r="R19" s="31">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I20" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I21" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N23" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="26">
         <f>SUM(E2:E6)</f>
         <v>99999.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N24" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31">
+        <f>SUM(R3:R7)</f>
+        <v>99999.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="26">
         <f>SUM(E8:E13)</f>
         <v>99960</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N25" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31">
+        <f>SUM(R8:R14)</f>
+        <v>99960</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="26">
         <f>SUM(E15:E18)</f>
         <v>100000</v>
+      </c>
+      <c r="N26" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31">
+        <f>SUM(R16:R19)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E27" s="26">
+        <f>SUM(E24:E26)</f>
+        <v>299959.8</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFCABA2-8D40-B74F-944B-94AF5E91C8C5}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -2974,11 +3372,11 @@
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4">
-        <f>$B39*D39</f>
+        <f t="shared" ref="H39:I41" si="4">$B39*D39</f>
         <v>112403.99999999999</v>
       </c>
       <c r="I39" s="4">
-        <f>$B39*E39</f>
+        <f t="shared" si="4"/>
         <v>112403.99999999999</v>
       </c>
       <c r="J39" s="10">
@@ -3028,15 +3426,15 @@
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4">
-        <f>$B40*D40</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I40" s="4">
-        <f>$B40*E40</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" ref="J40:J43" si="4">SUM(F40:I40)</f>
+        <f t="shared" ref="J40:J42" si="5">SUM(F40:I40)</f>
         <v>0</v>
       </c>
       <c r="K40" s="23"/>
@@ -3080,15 +3478,15 @@
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4">
-        <f>$B41*D41</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I41" s="4">
-        <f>$B41*E41</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J41" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K41" s="23"/>
@@ -3137,7 +3535,7 @@
         <v>20975.663999999997</v>
       </c>
       <c r="J42" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79834.991999999998</v>
       </c>
       <c r="K42" s="23"/>
@@ -3469,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" ref="I6:I9" si="1">SUM(F6:H6)</f>
+        <f t="shared" ref="I6:I8" si="1">SUM(F6:H6)</f>
         <v>0</v>
       </c>
       <c r="J6" s="4"/>

</xml_diff>